<commit_message>
revised hypo catalog format
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/catalog/hypo_catalog.xlsx
+++ b/tests/sample_tests_data/data/catalog/hypo_catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lqt-moment-magnitude\tests\sample_tests_data\catalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SEML\GITHUB DEPLOY\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDF4D1-23E8-4FDA-9E55-4B83D5200CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED52097B-3437-423E-B622-E09BAEDFF652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>elev_m</t>
+  </si>
+  <si>
+    <t>source_error_rms</t>
+  </si>
+  <si>
+    <t>n_phases</t>
+  </si>
+  <si>
+    <t>x_horizontal_err</t>
+  </si>
+  <si>
+    <t>y_horizontal_err</t>
+  </si>
+  <si>
+    <t>z_depth_err</t>
   </si>
 </sst>
 </file>
@@ -138,13 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,15 +482,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="18.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,11 +536,27 @@
       <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1001</v>
       </c>
@@ -558,10 +596,24 @@
       <c r="M2" s="5">
         <v>35.909999800000001</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N2" s="6">
+        <v>9.1886999999999993E-3</v>
+      </c>
+      <c r="O2" s="5">
+        <v>12</v>
+      </c>
+      <c r="P2" s="6">
+        <v>1081.373654200989</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>830.06207599191043</v>
+      </c>
+      <c r="R2" s="6">
+        <v>526.34828678357076</v>
+      </c>
+      <c r="T2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1002</v>
       </c>
@@ -601,10 +653,24 @@
       <c r="M3" s="5">
         <v>28.420000099999999</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N3" s="6">
+        <v>1.7569700000000001E-2</v>
+      </c>
+      <c r="O3" s="5">
+        <v>8</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1036.870449959878</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1110.1576824937979</v>
+      </c>
+      <c r="R3" s="6">
+        <v>572.14844577259839</v>
+      </c>
+      <c r="T3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1003</v>
       </c>
@@ -644,10 +710,24 @@
       <c r="M4" s="5">
         <v>6.7800001999999999</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N4" s="6">
+        <v>1.33344E-2</v>
+      </c>
+      <c r="O4" s="5">
+        <v>22</v>
+      </c>
+      <c r="P4" s="6">
+        <v>632.83370643479475</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>581.18210485182692</v>
+      </c>
+      <c r="R4" s="6">
+        <v>573.93518536503757</v>
+      </c>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1004</v>
       </c>
@@ -687,10 +767,24 @@
       <c r="M5" s="5">
         <v>4.0500002000000004</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N5" s="6">
+        <v>1.1108E-2</v>
+      </c>
+      <c r="O5" s="5">
+        <v>26</v>
+      </c>
+      <c r="P5" s="6">
+        <v>1061.4787656849289</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1026.8864202042989</v>
+      </c>
+      <c r="R5" s="6">
+        <v>602.83787206843601</v>
+      </c>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1005</v>
       </c>
@@ -730,52 +824,66 @@
       <c r="M6" s="5">
         <v>12.3800001</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N6" s="6">
+        <v>1.37886E-2</v>
+      </c>
+      <c r="O6" s="5">
+        <v>18</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1126.2873301249549</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1141.0111130046021</v>
+      </c>
+      <c r="R6" s="6">
+        <v>693.78431807010452</v>
+      </c>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more statistical attributes to the catalog
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/catalog/hypo_catalog.xlsx
+++ b/tests/sample_tests_data/data/catalog/hypo_catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SEML\GITHUB DEPLOY\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED52097B-3437-423E-B622-E09BAEDFF652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468A1014-52A1-420C-8B7D-17E1A561E02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -36,12 +36,6 @@
     <t>lon</t>
   </si>
   <si>
-    <t>utm_x</t>
-  </si>
-  <si>
-    <t>utm_y</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -66,22 +60,22 @@
     <t>depth_m</t>
   </si>
   <si>
-    <t>elev_m</t>
-  </si>
-  <si>
-    <t>source_error_rms</t>
-  </si>
-  <si>
     <t>n_phases</t>
   </si>
   <si>
-    <t>x_horizontal_err</t>
-  </si>
-  <si>
-    <t>y_horizontal_err</t>
-  </si>
-  <si>
-    <t>z_depth_err</t>
+    <t>gap_degree</t>
+  </si>
+  <si>
+    <t>source_err_rms_s</t>
+  </si>
+  <si>
+    <t>x_horizontal_err_m</t>
+  </si>
+  <si>
+    <t>y_horizontal_err_m</t>
+  </si>
+  <si>
+    <t>z_depth_err_m</t>
   </si>
 </sst>
 </file>
@@ -165,17 +159,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -482,21 +466,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="18.5703125" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,34 +491,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>14</v>
@@ -545,18 +529,11 @@
       <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1001</v>
       </c>
@@ -567,53 +544,46 @@
         <v>126.596433</v>
       </c>
       <c r="D2" s="5">
-        <v>289211.76</v>
+        <v>1252.26</v>
       </c>
       <c r="E2" s="5">
-        <v>4218348.0439999998</v>
+        <v>2024</v>
       </c>
       <c r="F2" s="5">
-        <v>1252.26</v>
+        <v>5</v>
       </c>
       <c r="G2" s="5">
-        <v>-1252.26</v>
+        <v>11</v>
       </c>
       <c r="H2" s="5">
-        <v>2024</v>
+        <v>15</v>
       </c>
       <c r="I2" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="J2" s="5">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5">
-        <v>15</v>
+        <v>35.909999800000001</v>
+      </c>
+      <c r="K2" s="6">
+        <v>9.1886999999999993E-3</v>
       </c>
       <c r="L2" s="5">
-        <v>30</v>
-      </c>
-      <c r="M2" s="5">
-        <v>35.909999800000001</v>
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>334.18700000000001</v>
       </c>
       <c r="N2" s="6">
-        <v>9.1886999999999993E-3</v>
-      </c>
-      <c r="O2" s="5">
-        <v>12</v>
+        <v>1081.373654200989</v>
+      </c>
+      <c r="O2" s="6">
+        <v>830.06207599191043</v>
       </c>
       <c r="P2" s="6">
-        <v>1081.373654200989</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>830.06207599191043</v>
-      </c>
-      <c r="R2" s="6">
         <v>526.34828678357076</v>
       </c>
-      <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1002</v>
       </c>
@@ -624,53 +594,46 @@
         <v>126.59125</v>
       </c>
       <c r="D3" s="5">
-        <v>288749.47860000003</v>
+        <v>1035.99</v>
       </c>
       <c r="E3" s="5">
-        <v>4218061.9859999996</v>
+        <v>2024</v>
       </c>
       <c r="F3" s="5">
-        <v>1035.99</v>
+        <v>5</v>
       </c>
       <c r="G3" s="5">
-        <v>-1035.99</v>
+        <v>11</v>
       </c>
       <c r="H3" s="5">
-        <v>2024</v>
+        <v>16</v>
       </c>
       <c r="I3" s="5">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="J3" s="5">
-        <v>11</v>
-      </c>
-      <c r="K3" s="5">
-        <v>16</v>
+        <v>28.420000099999999</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1.7569700000000001E-2</v>
       </c>
       <c r="L3" s="5">
-        <v>33</v>
-      </c>
-      <c r="M3" s="5">
-        <v>28.420000099999999</v>
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>336.02800000000002</v>
       </c>
       <c r="N3" s="6">
-        <v>1.7569700000000001E-2</v>
-      </c>
-      <c r="O3" s="5">
-        <v>8</v>
+        <v>1036.870449959878</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1110.1576824937979</v>
       </c>
       <c r="P3" s="6">
-        <v>1036.870449959878</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>1110.1576824937979</v>
-      </c>
-      <c r="R3" s="6">
         <v>572.14844577259839</v>
       </c>
-      <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1003</v>
       </c>
@@ -681,53 +644,46 @@
         <v>126.597537</v>
       </c>
       <c r="D4" s="5">
-        <v>289296.39850000001</v>
+        <v>705.16</v>
       </c>
       <c r="E4" s="5">
-        <v>4217872.5979999993</v>
+        <v>2024</v>
       </c>
       <c r="F4" s="5">
-        <v>705.16</v>
+        <v>5</v>
       </c>
       <c r="G4" s="5">
-        <v>-705.16</v>
+        <v>27</v>
       </c>
       <c r="H4" s="5">
-        <v>2024</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="J4" s="5">
-        <v>27</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1</v>
+        <v>6.7800001999999999</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1.33344E-2</v>
       </c>
       <c r="L4" s="5">
-        <v>19</v>
-      </c>
-      <c r="M4" s="5">
-        <v>6.7800001999999999</v>
+        <v>22</v>
+      </c>
+      <c r="M4">
+        <v>311.137</v>
       </c>
       <c r="N4" s="6">
-        <v>1.33344E-2</v>
-      </c>
-      <c r="O4" s="5">
-        <v>22</v>
+        <v>632.83370643479475</v>
+      </c>
+      <c r="O4" s="6">
+        <v>581.18210485182692</v>
       </c>
       <c r="P4" s="6">
-        <v>632.83370643479475</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>581.18210485182692</v>
-      </c>
-      <c r="R4" s="6">
         <v>573.93518536503757</v>
       </c>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1004</v>
       </c>
@@ -738,53 +694,46 @@
         <v>126.602059</v>
       </c>
       <c r="D5" s="5">
-        <v>289693.1409</v>
+        <v>770.66</v>
       </c>
       <c r="E5" s="5">
-        <v>4217867.6559999995</v>
+        <v>2024</v>
       </c>
       <c r="F5" s="5">
-        <v>770.66</v>
+        <v>5</v>
       </c>
       <c r="G5" s="5">
-        <v>-770.66</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5">
-        <v>2024</v>
+        <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J5" s="5">
-        <v>27</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1</v>
+        <v>4.0500002000000004</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1.1108E-2</v>
       </c>
       <c r="L5" s="5">
-        <v>20</v>
-      </c>
-      <c r="M5" s="5">
-        <v>4.0500002000000004</v>
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>336.71699999999998</v>
       </c>
       <c r="N5" s="6">
-        <v>1.1108E-2</v>
-      </c>
-      <c r="O5" s="5">
-        <v>26</v>
+        <v>1061.4787656849289</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1026.8864202042989</v>
       </c>
       <c r="P5" s="6">
-        <v>1061.4787656849289</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>1026.8864202042989</v>
-      </c>
-      <c r="R5" s="6">
         <v>602.83787206843601</v>
       </c>
-      <c r="T5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1005</v>
       </c>
@@ -795,118 +744,92 @@
         <v>126.59738900000001</v>
       </c>
       <c r="D6" s="5">
-        <v>289296.00930000003</v>
+        <v>1004.5</v>
       </c>
       <c r="E6" s="5">
-        <v>4218358.3389999997</v>
+        <v>2024</v>
       </c>
       <c r="F6" s="5">
-        <v>1004.5</v>
+        <v>5</v>
       </c>
       <c r="G6" s="5">
-        <v>-1004.5</v>
+        <v>27</v>
       </c>
       <c r="H6" s="5">
-        <v>2024</v>
+        <v>1</v>
       </c>
       <c r="I6" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5">
-        <v>27</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1</v>
+        <v>12.3800001</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1.37886E-2</v>
       </c>
       <c r="L6" s="5">
-        <v>21</v>
-      </c>
-      <c r="M6" s="5">
-        <v>12.3800001</v>
+        <v>18</v>
+      </c>
+      <c r="M6">
+        <v>341.58199999999999</v>
       </c>
       <c r="N6" s="6">
-        <v>1.37886E-2</v>
-      </c>
-      <c r="O6" s="5">
-        <v>18</v>
+        <v>1126.2873301249549</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1141.0111130046021</v>
       </c>
       <c r="P6" s="6">
-        <v>1126.2873301249549</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>1141.0111130046021</v>
-      </c>
-      <c r="R6" s="6">
         <v>693.78431807010452</v>
       </c>
-      <c r="T6" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F6">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="D2:D6">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>-1250</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="D11:D15">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>-1250</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
-      <formula>1250</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16:I20">
+  <conditionalFormatting sqref="F16:F20">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>-1250</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more docs tutor 1
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/catalog/hypo_catalog.xlsx
+++ b/tests/sample_tests_data/data/catalog/hypo_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SEML\GITHUB DEPLOY\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468A1014-52A1-420C-8B7D-17E1A561E02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945153C0-2853-41BD-B456-233C1B0CF6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>z_depth_err_m</t>
+  </si>
+  <si>
+    <t>source_id</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,55 +482,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>